<commit_message>
Assigning Location functions to testers.
</commit_message>
<xml_diff>
--- a/docs/UnitMapping.xlsx
+++ b/docs/UnitMapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\scott\source\repos\battleship\Java-Battleship\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14EF9535-71C3-4AD9-863D-0A7C6814B656}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42A0C92F-50AB-4558-AFF7-2B35FF49FE2E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{D0A5CAD9-D504-40E1-BDDA-964E7DB974D0}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{D0A5CAD9-D504-40E1-BDDA-964E7DB974D0}"/>
   </bookViews>
   <sheets>
     <sheet name="SW Units" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="93">
   <si>
     <t>SW Unit</t>
   </si>
@@ -296,6 +296,15 @@
   </si>
   <si>
     <t>toString()</t>
+  </si>
+  <si>
+    <t>Mel</t>
+  </si>
+  <si>
+    <t>Scott</t>
+  </si>
+  <si>
+    <t>Nick</t>
   </si>
 </sst>
 </file>
@@ -378,6 +387,9 @@
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -391,9 +403,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -718,7 +727,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70B92B2B-13D2-4BF6-94D0-AC46ADFF20BC}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -814,9 +825,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D6E0CAC-13D0-434A-82CB-663C690197D0}">
   <dimension ref="A1:E69"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -844,7 +853,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B2" t="s">
@@ -856,9 +865,12 @@
       <c r="D2" t="s">
         <v>12</v>
       </c>
+      <c r="E2" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
+      <c r="A3" s="3"/>
       <c r="B3" t="s">
         <v>19</v>
       </c>
@@ -868,9 +880,12 @@
       <c r="D3" t="s">
         <v>12</v>
       </c>
+      <c r="E3" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
+      <c r="A4" s="3"/>
       <c r="B4" t="s">
         <v>20</v>
       </c>
@@ -880,9 +895,12 @@
       <c r="D4" t="s">
         <v>12</v>
       </c>
+      <c r="E4" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
+      <c r="A5" s="3"/>
       <c r="B5" t="s">
         <v>21</v>
       </c>
@@ -892,9 +910,12 @@
       <c r="D5" t="s">
         <v>12</v>
       </c>
+      <c r="E5" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
+      <c r="A6" s="3"/>
       <c r="B6" t="s">
         <v>22</v>
       </c>
@@ -904,9 +925,12 @@
       <c r="D6" t="s">
         <v>12</v>
       </c>
+      <c r="E6" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
+      <c r="A7" s="3"/>
       <c r="B7" t="s">
         <v>23</v>
       </c>
@@ -916,9 +940,12 @@
       <c r="D7" t="s">
         <v>12</v>
       </c>
+      <c r="E7" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
+      <c r="A8" s="3"/>
       <c r="B8" t="s">
         <v>24</v>
       </c>
@@ -928,9 +955,12 @@
       <c r="D8" t="s">
         <v>12</v>
       </c>
+      <c r="E8" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
+      <c r="A9" s="3"/>
       <c r="B9" t="s">
         <v>25</v>
       </c>
@@ -940,9 +970,12 @@
       <c r="D9" t="s">
         <v>12</v>
       </c>
+      <c r="E9" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
+      <c r="A10" s="3"/>
       <c r="B10" t="s">
         <v>26</v>
       </c>
@@ -952,9 +985,12 @@
       <c r="D10" t="s">
         <v>12</v>
       </c>
+      <c r="E10" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
+      <c r="A11" s="3"/>
       <c r="B11" t="s">
         <v>27</v>
       </c>
@@ -964,9 +1000,12 @@
       <c r="D11" t="s">
         <v>12</v>
       </c>
+      <c r="E11" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
+      <c r="A12" s="3"/>
       <c r="B12" t="s">
         <v>28</v>
       </c>
@@ -976,9 +1015,12 @@
       <c r="D12" t="s">
         <v>12</v>
       </c>
+      <c r="E12" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
+      <c r="A13" s="3"/>
       <c r="B13" t="s">
         <v>29</v>
       </c>
@@ -988,9 +1030,12 @@
       <c r="D13" t="s">
         <v>12</v>
       </c>
+      <c r="E13" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
+      <c r="A14" s="3"/>
       <c r="B14" t="s">
         <v>30</v>
       </c>
@@ -1000,9 +1045,12 @@
       <c r="D14" t="s">
         <v>12</v>
       </c>
+      <c r="E14" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
+      <c r="A15" s="3"/>
       <c r="B15" t="s">
         <v>31</v>
       </c>
@@ -1012,9 +1060,12 @@
       <c r="D15" t="s">
         <v>12</v>
       </c>
+      <c r="E15" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B16" t="s">
@@ -1028,7 +1079,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="3"/>
+      <c r="A17" s="4"/>
       <c r="B17" t="s">
         <v>34</v>
       </c>
@@ -1040,7 +1091,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
+      <c r="A18" s="4"/>
       <c r="B18" t="s">
         <v>35</v>
       </c>
@@ -1052,7 +1103,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="3"/>
+      <c r="A19" s="4"/>
       <c r="B19" t="s">
         <v>36</v>
       </c>
@@ -1064,7 +1115,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="3"/>
+      <c r="A20" s="4"/>
       <c r="B20" t="s">
         <v>37</v>
       </c>
@@ -1076,7 +1127,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="3"/>
+      <c r="A21" s="4"/>
       <c r="B21" t="s">
         <v>38</v>
       </c>
@@ -1088,7 +1139,7 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="3"/>
+      <c r="A22" s="4"/>
       <c r="B22" t="s">
         <v>39</v>
       </c>
@@ -1100,7 +1151,7 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="3"/>
+      <c r="A23" s="4"/>
       <c r="B23" t="s">
         <v>40</v>
       </c>
@@ -1112,7 +1163,7 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="3"/>
+      <c r="A24" s="4"/>
       <c r="B24" t="s">
         <v>41</v>
       </c>
@@ -1124,7 +1175,7 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="3"/>
+      <c r="A25" s="4"/>
       <c r="B25" t="s">
         <v>42</v>
       </c>
@@ -1136,7 +1187,7 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="3"/>
+      <c r="A26" s="4"/>
       <c r="B26" t="s">
         <v>43</v>
       </c>
@@ -1148,7 +1199,7 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="3"/>
+      <c r="A27" s="4"/>
       <c r="B27" t="s">
         <v>44</v>
       </c>
@@ -1160,7 +1211,7 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="3"/>
+      <c r="A28" s="4"/>
       <c r="B28" t="s">
         <v>45</v>
       </c>
@@ -1172,7 +1223,7 @@
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="3"/>
+      <c r="A29" s="4"/>
       <c r="B29" t="s">
         <v>46</v>
       </c>
@@ -1184,7 +1235,7 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="3"/>
+      <c r="A30" s="4"/>
       <c r="B30" t="s">
         <v>47</v>
       </c>
@@ -1196,7 +1247,7 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="3"/>
+      <c r="A31" s="4"/>
       <c r="B31" t="s">
         <v>48</v>
       </c>
@@ -1208,7 +1259,7 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="3"/>
+      <c r="A32" s="4"/>
       <c r="B32" t="s">
         <v>49</v>
       </c>
@@ -1220,7 +1271,7 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="3"/>
+      <c r="A33" s="4"/>
       <c r="B33" t="s">
         <v>50</v>
       </c>
@@ -1232,7 +1283,7 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="s">
+      <c r="A34" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B34" t="s">
@@ -1246,7 +1297,7 @@
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="4"/>
+      <c r="A35" s="5"/>
       <c r="B35" t="s">
         <v>53</v>
       </c>
@@ -1258,7 +1309,7 @@
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="4"/>
+      <c r="A36" s="5"/>
       <c r="B36" t="s">
         <v>54</v>
       </c>
@@ -1270,7 +1321,7 @@
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="4"/>
+      <c r="A37" s="5"/>
       <c r="B37" t="s">
         <v>55</v>
       </c>
@@ -1282,7 +1333,7 @@
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="4"/>
+      <c r="A38" s="5"/>
       <c r="B38" t="s">
         <v>56</v>
       </c>
@@ -1294,7 +1345,7 @@
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="4"/>
+      <c r="A39" s="5"/>
       <c r="B39" t="s">
         <v>57</v>
       </c>
@@ -1306,7 +1357,7 @@
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="4"/>
+      <c r="A40" s="5"/>
       <c r="B40" t="s">
         <v>58</v>
       </c>
@@ -1318,7 +1369,7 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="4"/>
+      <c r="A41" s="5"/>
       <c r="B41" t="s">
         <v>59</v>
       </c>
@@ -1330,7 +1381,7 @@
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="4"/>
+      <c r="A42" s="5"/>
       <c r="B42" t="s">
         <v>60</v>
       </c>
@@ -1342,7 +1393,7 @@
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="4"/>
+      <c r="A43" s="5"/>
       <c r="B43" t="s">
         <v>61</v>
       </c>
@@ -1354,7 +1405,7 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="4"/>
+      <c r="A44" s="5"/>
       <c r="B44" t="s">
         <v>62</v>
       </c>
@@ -1366,7 +1417,7 @@
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="5" t="s">
+      <c r="A45" s="6" t="s">
         <v>9</v>
       </c>
       <c r="B45" t="s">
@@ -1380,7 +1431,7 @@
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="5"/>
+      <c r="A46" s="6"/>
       <c r="B46" t="s">
         <v>64</v>
       </c>
@@ -1392,7 +1443,7 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="5"/>
+      <c r="A47" s="6"/>
       <c r="B47" t="s">
         <v>65</v>
       </c>
@@ -1404,7 +1455,7 @@
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="5"/>
+      <c r="A48" s="6"/>
       <c r="B48" t="s">
         <v>66</v>
       </c>
@@ -1416,7 +1467,7 @@
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="6" t="s">
+      <c r="A49" s="7" t="s">
         <v>6</v>
       </c>
       <c r="B49" t="s">
@@ -1430,7 +1481,7 @@
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="6"/>
+      <c r="A50" s="7"/>
       <c r="B50" t="s">
         <v>70</v>
       </c>
@@ -1442,7 +1493,7 @@
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="6"/>
+      <c r="A51" s="7"/>
       <c r="B51" t="s">
         <v>71</v>
       </c>
@@ -1454,7 +1505,7 @@
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="6"/>
+      <c r="A52" s="7"/>
       <c r="B52" t="s">
         <v>72</v>
       </c>
@@ -1466,7 +1517,7 @@
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="6"/>
+      <c r="A53" s="7"/>
       <c r="B53" t="s">
         <v>73</v>
       </c>
@@ -1478,7 +1529,7 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="6"/>
+      <c r="A54" s="7"/>
       <c r="B54" t="s">
         <v>74</v>
       </c>
@@ -1490,7 +1541,7 @@
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="6"/>
+      <c r="A55" s="7"/>
       <c r="B55" t="s">
         <v>75</v>
       </c>
@@ -1502,7 +1553,7 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="6"/>
+      <c r="A56" s="7"/>
       <c r="B56" t="s">
         <v>76</v>
       </c>
@@ -1514,7 +1565,7 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="6"/>
+      <c r="A57" s="7"/>
       <c r="B57" t="s">
         <v>77</v>
       </c>
@@ -1526,7 +1577,7 @@
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="6"/>
+      <c r="A58" s="7"/>
       <c r="B58" t="s">
         <v>78</v>
       </c>
@@ -1538,7 +1589,7 @@
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="7" t="s">
+      <c r="A59" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B59" t="s">
@@ -1552,7 +1603,7 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="7"/>
+      <c r="A60" s="2"/>
       <c r="B60" t="s">
         <v>80</v>
       </c>
@@ -1564,7 +1615,7 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="7"/>
+      <c r="A61" s="2"/>
       <c r="B61" t="s">
         <v>81</v>
       </c>
@@ -1576,7 +1627,7 @@
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="7"/>
+      <c r="A62" s="2"/>
       <c r="B62" t="s">
         <v>82</v>
       </c>
@@ -1588,7 +1639,7 @@
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="7"/>
+      <c r="A63" s="2"/>
       <c r="B63" t="s">
         <v>83</v>
       </c>
@@ -1600,7 +1651,7 @@
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="7"/>
+      <c r="A64" s="2"/>
       <c r="B64" t="s">
         <v>84</v>
       </c>
@@ -1612,7 +1663,7 @@
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="7"/>
+      <c r="A65" s="2"/>
       <c r="B65" t="s">
         <v>85</v>
       </c>
@@ -1624,7 +1675,7 @@
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="7"/>
+      <c r="A66" s="2"/>
       <c r="B66" t="s">
         <v>86</v>
       </c>
@@ -1636,7 +1687,7 @@
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="7"/>
+      <c r="A67" s="2"/>
       <c r="B67" t="s">
         <v>87</v>
       </c>
@@ -1648,7 +1699,7 @@
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="7"/>
+      <c r="A68" s="2"/>
       <c r="B68" t="s">
         <v>88</v>
       </c>
@@ -1660,7 +1711,7 @@
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="7"/>
+      <c r="A69" s="2"/>
       <c r="B69" t="s">
         <v>89</v>
       </c>

</xml_diff>

<commit_message>
Updating SW unit mapping spreadsheet.
</commit_message>
<xml_diff>
--- a/docs/UnitMapping.xlsx
+++ b/docs/UnitMapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\scott\source\repos\battleship\Java-Battleship\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42A0C92F-50AB-4558-AFF7-2B35FF49FE2E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C382F5BD-0A99-483E-B42E-EBD471B0153B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{D0A5CAD9-D504-40E1-BDDA-964E7DB974D0}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="95">
   <si>
     <t>SW Unit</t>
   </si>
@@ -305,6 +305,12 @@
   </si>
   <si>
     <t>Nick</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Status</t>
   </si>
 </sst>
 </file>
@@ -823,7 +829,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D6E0CAC-13D0-434A-82CB-663C690197D0}">
-  <dimension ref="A1:E69"/>
+  <dimension ref="A1:F69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -835,7 +841,7 @@
     <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -851,8 +857,11 @@
       <c r="E1" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>11</v>
       </c>
@@ -868,8 +877,11 @@
       <c r="E2" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" t="s">
         <v>19</v>
@@ -883,8 +895,11 @@
       <c r="E3" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" t="s">
         <v>20</v>
@@ -898,8 +913,11 @@
       <c r="E4" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" t="s">
         <v>21</v>
@@ -913,8 +931,11 @@
       <c r="E5" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" t="s">
         <v>22</v>
@@ -928,8 +949,11 @@
       <c r="E6" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" t="s">
         <v>23</v>
@@ -943,8 +967,11 @@
       <c r="E7" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" t="s">
         <v>24</v>
@@ -958,8 +985,11 @@
       <c r="E8" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" t="s">
         <v>25</v>
@@ -973,8 +1003,11 @@
       <c r="E9" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" t="s">
         <v>26</v>
@@ -988,8 +1021,11 @@
       <c r="E10" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F10" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" t="s">
         <v>27</v>
@@ -1003,8 +1039,11 @@
       <c r="E11" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F11" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" t="s">
         <v>28</v>
@@ -1018,8 +1057,11 @@
       <c r="E12" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F12" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" t="s">
         <v>29</v>
@@ -1033,8 +1075,11 @@
       <c r="E13" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F13" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" t="s">
         <v>30</v>
@@ -1048,8 +1093,11 @@
       <c r="E14" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F14" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" t="s">
         <v>31</v>
@@ -1063,8 +1111,11 @@
       <c r="E15" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F15" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
Updating unit mapping spreadsheet.
</commit_message>
<xml_diff>
--- a/docs/UnitMapping.xlsx
+++ b/docs/UnitMapping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\scott\source\repos\battleship\Java-Battleship\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Scott\source\repos\BattleShip\Java-Battleship\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C382F5BD-0A99-483E-B42E-EBD471B0153B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB56CC1C-F6F3-4797-8E0C-E4739C4FCC0D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{D0A5CAD9-D504-40E1-BDDA-964E7DB974D0}"/>
+    <workbookView xWindow="13550" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{D0A5CAD9-D504-40E1-BDDA-964E7DB974D0}"/>
   </bookViews>
   <sheets>
     <sheet name="SW Units" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="96">
   <si>
     <t>SW Unit</t>
   </si>
@@ -67,9 +67,6 @@
     <t>Yes</t>
   </si>
   <si>
-    <t>Too simple?</t>
-  </si>
-  <si>
     <t>Most return types are boolean</t>
   </si>
   <si>
@@ -311,6 +308,12 @@
   </si>
   <si>
     <t>Status</t>
+  </si>
+  <si>
+    <t>Melissa</t>
+  </si>
+  <si>
+    <t>?</t>
   </si>
 </sst>
 </file>
@@ -733,9 +736,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70B92B2B-13D2-4BF6-94D0-AC46ADFF20BC}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
-    </sheetView>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -784,9 +785,6 @@
       <c r="B4" t="s">
         <v>12</v>
       </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -795,9 +793,6 @@
       <c r="B5" t="s">
         <v>12</v>
       </c>
-      <c r="C5" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -807,7 +802,7 @@
         <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -818,7 +813,7 @@
         <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -831,7 +826,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D6E0CAC-13D0-434A-82CB-663C690197D0}">
   <dimension ref="A1:F69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -843,22 +838,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -866,253 +861,253 @@
         <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D2" t="s">
         <v>12</v>
       </c>
       <c r="E2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D3" t="s">
         <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D4" t="s">
         <v>12</v>
       </c>
       <c r="E4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
       </c>
       <c r="E5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D6" t="s">
         <v>12</v>
       </c>
       <c r="E6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D7" t="s">
         <v>12</v>
       </c>
       <c r="E7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D8" t="s">
         <v>12</v>
       </c>
       <c r="E8" t="s">
+        <v>91</v>
+      </c>
+      <c r="F8" t="s">
         <v>92</v>
-      </c>
-      <c r="F8" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D9" t="s">
         <v>12</v>
       </c>
       <c r="E9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D10" t="s">
         <v>12</v>
       </c>
       <c r="E10" t="s">
+        <v>91</v>
+      </c>
+      <c r="F10" t="s">
         <v>92</v>
-      </c>
-      <c r="F10" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D11" t="s">
         <v>12</v>
       </c>
       <c r="E11" t="s">
+        <v>91</v>
+      </c>
+      <c r="F11" t="s">
         <v>92</v>
-      </c>
-      <c r="F11" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D12" t="s">
         <v>12</v>
       </c>
       <c r="E12" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D13" t="s">
         <v>12</v>
       </c>
       <c r="E13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D14" t="s">
         <v>12</v>
       </c>
       <c r="E14" t="s">
+        <v>91</v>
+      </c>
+      <c r="F14" t="s">
         <v>92</v>
-      </c>
-      <c r="F14" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D15" t="s">
         <v>12</v>
       </c>
       <c r="E15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F15" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -1120,657 +1115,837 @@
         <v>10</v>
       </c>
       <c r="B16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D16" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C17" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D17" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D18" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D19" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C20" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D20" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E20" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D21" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E21" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C22" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D22" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E22" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C23" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D23" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E23" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C24" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D24" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E24" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C25" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D25" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E25" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C26" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D26" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E26" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C27" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D27" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E27" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D28" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E28" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C29" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D29" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E29" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C30" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D30" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E30" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D31" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E31" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="B32" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C32" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D32" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E32" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
       <c r="B33" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C33" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D33" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E33" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B34" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C34" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D34" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E34" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="5"/>
       <c r="B35" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C35" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D35" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E35" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="5"/>
       <c r="B36" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C36" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D36" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E36" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="5"/>
       <c r="B37" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C37" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D37" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E37" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="5"/>
       <c r="B38" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C38" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D38" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E38" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="5"/>
       <c r="B39" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C39" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D39" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E39" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="5"/>
       <c r="B40" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C40" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D40" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E40" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="5"/>
       <c r="B41" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C41" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D41" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E41" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="5"/>
       <c r="B42" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C42" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D42" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E42" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="5"/>
       <c r="B43" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C43" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D43" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E43" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="5"/>
       <c r="B44" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C44" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D44" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E44" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
         <v>9</v>
       </c>
       <c r="B45" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C45" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D45" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E45" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="6"/>
       <c r="B46" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C46" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D46" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E46" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="6"/>
       <c r="B47" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C47" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D47" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E47" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="6"/>
       <c r="B48" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C48" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D48" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E48" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
         <v>6</v>
       </c>
       <c r="B49" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C49" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D49" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E49" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="7"/>
       <c r="B50" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C50" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D50" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E50" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="7"/>
       <c r="B51" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C51" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D51" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E51" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="7"/>
       <c r="B52" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C52" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D52" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E52" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="7"/>
       <c r="B53" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C53" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D53" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E53" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="7"/>
       <c r="B54" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C54" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D54" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E54" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="7"/>
       <c r="B55" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C55" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D55" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E55" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="7"/>
       <c r="B56" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C56" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D56" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E56" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="7"/>
       <c r="B57" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C57" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D57" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E57" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="7"/>
       <c r="B58" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C58" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D58" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E58" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B59" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C59" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D59" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E59" t="s">
+        <v>91</v>
+      </c>
+      <c r="F59" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="2"/>
       <c r="B60" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C60" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D60" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E60" t="s">
+        <v>91</v>
+      </c>
+      <c r="F60" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="2"/>
       <c r="B61" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C61" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D61" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E61" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="2"/>
       <c r="B62" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C62" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D62" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E62" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="2"/>
       <c r="B63" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C63" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D63" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E63" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="2"/>
       <c r="B64" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C64" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D64" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E64" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="2"/>
       <c r="B65" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C65" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D65" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E65" t="s">
+        <v>91</v>
+      </c>
+      <c r="F65" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="2"/>
       <c r="B66" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C66" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D66" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E66" t="s">
+        <v>91</v>
+      </c>
+      <c r="F66" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="2"/>
       <c r="B67" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C67" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D67" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E67" t="s">
+        <v>91</v>
+      </c>
+      <c r="F67" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="2"/>
       <c r="B68" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C68" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D68" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E68" t="s">
+        <v>91</v>
+      </c>
+      <c r="F68" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="2"/>
       <c r="B69" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C69" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D69" t="s">
         <v>12</v>
+      </c>
+      <c r="E69" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>